<commit_message>
improved settings xlsx and made backup in tmp/
</commit_message>
<xml_diff>
--- a/comparison-cpb-uwv.xlsx
+++ b/comparison-cpb-uwv.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mdijkstra/Dropbox/cpb/git/szu/prijsvgl/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\p_onderhoud_mimosi_macro\Test_prijsvergelijking\Test3\szu-monitor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1981CF3-14B7-FD45-9AF3-E92988C8EF04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DC69A43-F661-4718-BF84-7950D1C87BDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{C245FD2E-A8EF-FE49-BCB6-6A57B2A0977F}"/>
+    <workbookView xWindow="2820" yWindow="1620" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{C245FD2E-A8EF-FE49-BCB6-6A57B2A0977F}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -44,9 +44,6 @@
     <t>file_mut</t>
   </si>
   <si>
-    <t>m:/p_onderhoud_mimosi_macro/mpp/mpp_data_out_02/mpp_02_2024_uwv (nota 2024m06) mon.xlsx; input/uwv-nota-2024-06.xlsx</t>
-  </si>
-  <si>
     <t>run</t>
   </si>
   <si>
@@ -233,18 +230,12 @@
     <t>whk_wga_wn / whk_wga_mn - whk_wga_wn_uwv / whk_wga_mn_uwv</t>
   </si>
   <si>
-    <t>whk_zw_wn / whk_zw_mn - whk_zw_wn_uwv / whk_zw_wn_uwv</t>
-  </si>
-  <si>
     <t>erd_wga_wn / erd_wga_mn - erd_wga_wn_uwv / erd_wga_mn_uwv</t>
   </si>
   <si>
     <t>wajong_wn / wajong_mn - wajong_wn_uwv / wajong_mn_uwv</t>
   </si>
   <si>
-    <t>awf_ww_wn / awf_ww_mn - (awf_ww_wn_uwv + awf_wwown_uwv) / (awf_ww_mn_uwv + awf_wwown_uwv)</t>
-  </si>
-  <si>
     <t>awf_zw_wn / awf_zw_mn - afw_zw_wn_uwv / awf_zw_mn_uwv</t>
   </si>
   <si>
@@ -1082,13 +1073,44 @@
   </si>
   <si>
     <t>output/mut_${run_mimosi}_wage-related.xlsx</t>
+  </si>
+  <si>
+    <t>m:/p_onderhoud_mimosi_macro/mpp/mpp_data_out_02/mpp_02_2024_uwv (nota 2024m06 concept) mon.xlsx</t>
+  </si>
+  <si>
+    <r>
+      <t>whk_zw_wn / whk_zw_mn - whk_zw_wn_uwv / whk_zw_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>m</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>n_uwv</t>
+    </r>
+  </si>
+  <si>
+    <t>awf_ww_wn / awf_ww_mn - (awf_ww_wn_uwv + awf_wwown_uwv) / (awf_ww_mn_uwv)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1101,6 +1123,7 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1108,6 +1131,7 @@
       <sz val="12"/>
       <color theme="0" tint="-0.499984740745262"/>
       <name val="Aptos Narrow"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1133,11 +1157,13 @@
       <sz val="12"/>
       <color theme="8"/>
       <name val="Aptos Narrow"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <name val="Aptos Narrow"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1146,8 +1172,15 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1172,6 +1205,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1185,7 +1224,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1204,6 +1243,8 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1540,336 +1581,336 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88B2B392-A322-7F4B-BA28-5AA75E98CDC4}">
   <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="155" zoomScaleNormal="155" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView topLeftCell="A4" zoomScale="155" zoomScaleNormal="155" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="36.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="66.1640625" customWidth="1"/>
-    <col min="3" max="3" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.625" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="66.125" customWidth="1"/>
+    <col min="3" max="3" width="4.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" s="13" customFormat="1">
       <c r="A1" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="C1" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="D1" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="D1" s="12" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="11" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="14" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="15">
         <v>661</v>
       </c>
       <c r="D3" s="3"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4">
       <c r="A4" s="14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4" s="15">
         <v>2024</v>
       </c>
       <c r="D4" s="3"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4">
       <c r="A5" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D5" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="6" t="s">
+      <c r="C6" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>6</v>
-      </c>
       <c r="C7" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" s="6" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D8" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" s="6" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B9" s="4">
         <v>150</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4">
       <c r="A11" s="11" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="C13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="B12" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="C12" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="B13" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="C13" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="11" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:4">
       <c r="A16" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B16">
         <f>B3+1</f>
         <v>662</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="B17" t="s">
+        <v>132</v>
+      </c>
+      <c r="C17" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="B18" s="10" t="s">
         <v>144</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C18" s="4"/>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="B21" t="s">
+        <v>131</v>
+      </c>
+      <c r="C21" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="C17" t="s">
+      <c r="B22" t="s">
+        <v>138</v>
+      </c>
+      <c r="C22" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="B23" t="s">
+        <v>139</v>
+      </c>
+      <c r="C23" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="B24" t="s">
+        <v>146</v>
+      </c>
+      <c r="C24" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="B25" t="s">
+        <v>134</v>
+      </c>
+      <c r="C25" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="B18" s="10" t="s">
-        <v>147</v>
-      </c>
-      <c r="C18" s="4"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="B21" t="s">
-        <v>134</v>
-      </c>
-      <c r="C21" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="B22" t="s">
-        <v>141</v>
-      </c>
-      <c r="C22" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="B23" t="s">
-        <v>142</v>
-      </c>
-      <c r="C23" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="B24" t="s">
-        <v>149</v>
-      </c>
-      <c r="C24" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="B25" t="s">
-        <v>137</v>
-      </c>
-      <c r="C25" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4">
       <c r="A27" s="1" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
       <c r="A28" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B28" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
       <c r="A29" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B29" t="s">
+        <v>52</v>
+      </c>
+      <c r="D29" t="s">
         <v>51</v>
       </c>
-      <c r="B29" t="s">
-        <v>53</v>
-      </c>
-      <c r="D29" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="31" spans="1:4">
       <c r="A31" s="1" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
       <c r="A32" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="B32" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="B33" t="s">
+        <v>158</v>
+      </c>
+      <c r="C33" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="B34" t="s">
+        <v>151</v>
+      </c>
+      <c r="C34" t="s">
+        <v>37</v>
+      </c>
+      <c r="D34" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="6" t="s">
         <v>150</v>
       </c>
-      <c r="B32" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="B33" t="s">
-        <v>161</v>
-      </c>
-      <c r="C33" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" s="6" t="s">
+      <c r="B35" t="s">
+        <v>151</v>
+      </c>
+      <c r="C35" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="B36" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="B37" t="s">
         <v>152</v>
       </c>
-      <c r="B34" t="s">
-        <v>154</v>
-      </c>
-      <c r="C34" t="s">
-        <v>38</v>
-      </c>
-      <c r="D34" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="B35" t="s">
-        <v>154</v>
-      </c>
-      <c r="C35" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" s="6" t="s">
-        <v>157</v>
-      </c>
-      <c r="B36" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" s="6" t="s">
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="B38" t="s">
         <v>156</v>
-      </c>
-      <c r="B37" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" s="6" t="s">
-        <v>158</v>
-      </c>
-      <c r="B38" t="s">
-        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -1881,253 +1922,255 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26890EA4-2B43-0440-8F56-0827FAF291B4}">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView zoomScale="149" zoomScaleNormal="149" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="149" zoomScaleNormal="149" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="6.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="123.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="123.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" s="2" customFormat="1">
       <c r="A1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>46</v>
-      </c>
       <c r="C1" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" t="s">
         <v>57</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="D2" s="8" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B7" t="s">
         <v>20</v>
       </c>
-      <c r="C2" t="s">
-        <v>58</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="C7" t="s">
+        <v>62</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="16" customFormat="1">
+      <c r="A8" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" t="s">
-        <v>59</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="B8" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="C5" t="s">
-        <v>61</v>
-      </c>
-      <c r="D5" s="8" t="s">
+      <c r="C8" s="16" t="s">
+        <v>164</v>
+      </c>
+      <c r="D8" s="17" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" t="s">
-        <v>62</v>
-      </c>
-      <c r="D6" s="8" t="s">
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" t="s">
+        <v>63</v>
+      </c>
+      <c r="D9" s="8" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" t="s">
+    <row r="10" spans="1:4" s="16" customFormat="1">
+      <c r="A10" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" s="16" customFormat="1">
+      <c r="A11" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="C7" t="s">
-        <v>63</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" t="s">
-        <v>64</v>
-      </c>
-      <c r="D8" s="8" t="s">
+      <c r="C11" s="16" t="s">
+        <v>165</v>
+      </c>
+      <c r="D11" s="17" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" t="s">
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" t="s">
         <v>65</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D12" s="8" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" t="s">
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="8"/>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="8"/>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" s="8"/>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" t="s">
         <v>66</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D16" s="8" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" t="s">
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" t="s">
         <v>22</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C17" t="s">
         <v>67</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D17" s="8" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" t="s">
-        <v>68</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
         <v>13</v>
       </c>
-      <c r="B13" t="s">
-        <v>22</v>
-      </c>
-      <c r="D13" s="8"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
+      <c r="B18" t="s">
         <v>23</v>
       </c>
-      <c r="D14" s="8"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" t="s">
-        <v>24</v>
-      </c>
-      <c r="D15" s="8"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="D18" s="8"/>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
         <v>14</v>
       </c>
-      <c r="B16" t="s">
-        <v>22</v>
-      </c>
-      <c r="C16" t="s">
-        <v>69</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+      <c r="B19" t="s">
         <v>14</v>
-      </c>
-      <c r="B17" t="s">
-        <v>23</v>
-      </c>
-      <c r="C17" t="s">
-        <v>70</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>14</v>
-      </c>
-      <c r="B18" t="s">
-        <v>24</v>
-      </c>
-      <c r="D18" s="8"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>15</v>
-      </c>
-      <c r="B19" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -2143,252 +2186,252 @@
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="6.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" s="2" customFormat="1">
       <c r="A1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>46</v>
-      </c>
       <c r="C1" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>111</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>112</v>
+      </c>
+      <c r="D4" s="7" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
+        <v>114</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B7" t="s">
         <v>20</v>
       </c>
-      <c r="C2" t="s">
-        <v>113</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="C7" t="s">
+        <v>115</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" t="s">
-        <v>114</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" t="s">
-        <v>115</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="B8" t="s">
         <v>18</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C8" t="s">
         <v>116</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D8" s="7" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" t="s">
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" t="s">
         <v>117</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D9" s="7" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" t="s">
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" t="s">
+        <v>118</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
         <v>21</v>
       </c>
-      <c r="C7" t="s">
-        <v>118</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="C11" t="s">
         <v>119</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D11" s="7" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" t="s">
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" t="s">
         <v>120</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D12" s="7" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" t="s">
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="7"/>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="7"/>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" s="7"/>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" t="s">
         <v>121</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D16" s="7" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" t="s">
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" t="s">
         <v>22</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C17" t="s">
         <v>122</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D17" s="7" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" t="s">
-        <v>123</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
         <v>13</v>
       </c>
-      <c r="B13" t="s">
-        <v>22</v>
-      </c>
-      <c r="D13" s="7"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
+      <c r="B18" t="s">
         <v>23</v>
       </c>
-      <c r="D14" s="7"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" t="s">
-        <v>24</v>
-      </c>
-      <c r="D15" s="7"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="D18" s="7"/>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
         <v>14</v>
       </c>
-      <c r="B16" t="s">
-        <v>22</v>
-      </c>
-      <c r="C16" t="s">
-        <v>124</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+      <c r="B19" t="s">
         <v>14</v>
-      </c>
-      <c r="B17" t="s">
-        <v>23</v>
-      </c>
-      <c r="C17" t="s">
-        <v>125</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>14</v>
-      </c>
-      <c r="B18" t="s">
-        <v>24</v>
-      </c>
-      <c r="D18" s="7"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>15</v>
-      </c>
-      <c r="B19" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -2404,248 +2447,248 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="6.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="82.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="82.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" s="2" customFormat="1">
       <c r="A1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>46</v>
-      </c>
       <c r="C1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="D1" s="5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B7" t="s">
         <v>20</v>
       </c>
-      <c r="C2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="C7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D3" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="B8" t="s">
         <v>18</v>
       </c>
-      <c r="C5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="C8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D6" t="s">
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" t="s">
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
         <v>21</v>
       </c>
-      <c r="C7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D7" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="C11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" t="s">
-        <v>32</v>
-      </c>
-      <c r="D9" t="s">
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" t="s">
-        <v>37</v>
-      </c>
-      <c r="D10" t="s">
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" t="s">
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" t="s">
         <v>22</v>
       </c>
-      <c r="C11" t="s">
-        <v>33</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="C17" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" t="s">
-        <v>34</v>
-      </c>
-      <c r="D12" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
         <v>13</v>
       </c>
-      <c r="B13" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
+      <c r="B18" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
         <v>14</v>
       </c>
-      <c r="B16" t="s">
-        <v>22</v>
-      </c>
-      <c r="C16" t="s">
-        <v>35</v>
-      </c>
-      <c r="D16" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+      <c r="B19" t="s">
         <v>14</v>
-      </c>
-      <c r="B17" t="s">
-        <v>23</v>
-      </c>
-      <c r="C17" t="s">
-        <v>36</v>
-      </c>
-      <c r="D17" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>14</v>
-      </c>
-      <c r="B18" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>15</v>
-      </c>
-      <c r="B19" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
move tab mutdata to front
</commit_message>
<xml_diff>
--- a/comparison-cpb-uwv.xlsx
+++ b/comparison-cpb-uwv.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\p_onderhoud_mimosi_macro\Test_prijsvergelijking\Test3\szu-monitor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mdijkstra/Dropbox/cpb/git/szu/prijsvgl/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DC69A43-F661-4718-BF84-7950D1C87BDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D253A4C-0875-C440-B08B-7244357805AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2820" yWindow="1620" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{C245FD2E-A8EF-FE49-BCB6-6A57B2A0977F}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="34560" windowHeight="21100" xr2:uid="{C245FD2E-A8EF-FE49-BCB6-6A57B2A0977F}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -1075,9 +1075,6 @@
     <t>output/mut_${run_mimosi}_wage-related.xlsx</t>
   </si>
   <si>
-    <t>m:/p_onderhoud_mimosi_macro/mpp/mpp_data_out_02/mpp_02_2024_uwv (nota 2024m06 concept) mon.xlsx</t>
-  </si>
-  <si>
     <r>
       <t>whk_zw_wn / whk_zw_mn - whk_zw_wn_uwv / whk_zw_</t>
     </r>
@@ -1104,13 +1101,16 @@
   </si>
   <si>
     <t>awf_ww_wn / awf_ww_mn - (awf_ww_wn_uwv + awf_wwown_uwv) / (awf_ww_mn_uwv)</t>
+  </si>
+  <si>
+    <t>m:/p_onderhoud_mimosi_macro/mpp/mpp_data_out_02/mpp_02_2024_uwv (nota 2024m06 concept) mon.xlsx; input/uwv-nota-2024-06-sociale-lasten.xlsx</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1581,18 +1581,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88B2B392-A322-7F4B-BA28-5AA75E98CDC4}">
   <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="155" zoomScaleNormal="155" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="155" zoomScaleNormal="155" workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="36.625" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="66.125" customWidth="1"/>
-    <col min="3" max="3" width="4.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="66.1640625" customWidth="1"/>
+    <col min="3" max="3" width="4.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="13" customFormat="1">
+    <row r="1" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
         <v>46</v>
       </c>
@@ -1606,12 +1606,12 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
         <v>1</v>
       </c>
@@ -1620,7 +1620,7 @@
       </c>
       <c r="D3" s="3"/>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
         <v>8</v>
       </c>
@@ -1629,7 +1629,7 @@
       </c>
       <c r="D4" s="3"/>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>39</v>
       </c>
@@ -1640,7 +1640,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>41</v>
       </c>
@@ -1651,7 +1651,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>42</v>
       </c>
@@ -1662,7 +1662,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>124</v>
       </c>
@@ -1676,7 +1676,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>142</v>
       </c>
@@ -1688,16 +1688,16 @@
         <v>143</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="14" t="s">
         <v>123</v>
       </c>
@@ -1708,23 +1708,23 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="14" t="s">
         <v>40</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="C13" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="11" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
         <v>53</v>
       </c>
@@ -1736,7 +1736,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
         <v>141</v>
       </c>
@@ -1747,7 +1747,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
         <v>145</v>
       </c>
@@ -1756,12 +1756,12 @@
       </c>
       <c r="C18" s="4"/>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
         <v>130</v>
       </c>
@@ -1772,7 +1772,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
         <v>135</v>
       </c>
@@ -1783,7 +1783,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
         <v>136</v>
       </c>
@@ -1794,7 +1794,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
         <v>140</v>
       </c>
@@ -1805,7 +1805,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
         <v>133</v>
       </c>
@@ -1816,12 +1816,12 @@
         <v>38</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="s">
         <v>0</v>
       </c>
@@ -1829,7 +1829,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
         <v>50</v>
       </c>
@@ -1840,12 +1840,12 @@
         <v>51</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="6" t="s">
         <v>147</v>
       </c>
@@ -1853,7 +1853,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="6" t="s">
         <v>157</v>
       </c>
@@ -1864,7 +1864,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="6" t="s">
         <v>149</v>
       </c>
@@ -1878,7 +1878,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="6" t="s">
         <v>150</v>
       </c>
@@ -1889,7 +1889,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="6" t="s">
         <v>154</v>
       </c>
@@ -1897,7 +1897,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="6" t="s">
         <v>153</v>
       </c>
@@ -1905,7 +1905,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="6" t="s">
         <v>155</v>
       </c>
@@ -1922,18 +1922,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26890EA4-2B43-0440-8F56-0827FAF291B4}">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="149" zoomScaleNormal="149" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScale="149" zoomScaleNormal="149" workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="123.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="123.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1">
+    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>44</v>
       </c>
@@ -1947,7 +1947,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1961,7 +1961,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1975,7 +1975,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1989,7 +1989,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -2003,7 +2003,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -2017,7 +2017,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -2031,7 +2031,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="8" spans="1:4" s="16" customFormat="1">
+    <row r="8" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="16" t="s">
         <v>7</v>
       </c>
@@ -2039,13 +2039,13 @@
         <v>18</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D8" s="17" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -2059,7 +2059,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="16" customFormat="1">
+    <row r="10" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="16" t="s">
         <v>10</v>
       </c>
@@ -2073,7 +2073,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="11" spans="1:4" s="16" customFormat="1">
+    <row r="11" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="16" t="s">
         <v>11</v>
       </c>
@@ -2081,13 +2081,13 @@
         <v>21</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D11" s="17" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -2101,7 +2101,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -2110,7 +2110,7 @@
       </c>
       <c r="D13" s="8"/>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -2119,7 +2119,7 @@
       </c>
       <c r="D14" s="8"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -2128,7 +2128,7 @@
       </c>
       <c r="D15" s="8"/>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -2142,7 +2142,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -2156,7 +2156,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>13</v>
       </c>
@@ -2165,7 +2165,7 @@
       </c>
       <c r="D18" s="8"/>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>14</v>
       </c>
@@ -2186,15 +2186,15 @@
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1">
+    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>44</v>
       </c>
@@ -2208,7 +2208,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -2222,7 +2222,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -2236,7 +2236,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -2250,7 +2250,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -2264,7 +2264,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -2278,7 +2278,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -2292,7 +2292,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -2306,7 +2306,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -2320,7 +2320,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -2334,7 +2334,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -2348,7 +2348,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -2362,7 +2362,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -2371,7 +2371,7 @@
       </c>
       <c r="D13" s="7"/>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -2380,7 +2380,7 @@
       </c>
       <c r="D14" s="7"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -2389,7 +2389,7 @@
       </c>
       <c r="D15" s="7"/>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -2403,7 +2403,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -2417,7 +2417,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>13</v>
       </c>
@@ -2426,7 +2426,7 @@
       </c>
       <c r="D18" s="7"/>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>14</v>
       </c>
@@ -2447,15 +2447,15 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="82.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="82.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1">
+    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>44</v>
       </c>
@@ -2469,7 +2469,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -2483,7 +2483,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -2497,7 +2497,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -2511,7 +2511,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -2525,7 +2525,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -2539,7 +2539,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -2553,7 +2553,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -2567,7 +2567,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -2581,7 +2581,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -2595,7 +2595,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -2609,7 +2609,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -2623,7 +2623,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -2631,7 +2631,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -2639,7 +2639,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -2647,7 +2647,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -2661,7 +2661,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -2675,7 +2675,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>13</v>
       </c>
@@ -2683,7 +2683,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>14</v>
       </c>

</xml_diff>